<commit_message>
validata procedura di aggiornamento della distribuzione di probabilità del parametro Confidence
</commit_message>
<xml_diff>
--- a/Grid Planner/lib/SARLib/Toolbox/analisi propagazione confidenza.xlsx
+++ b/Grid Planner/lib/SARLib/Toolbox/analisi propagazione confidenza.xlsx
@@ -294,124 +294,124 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>0.64</c:v>
+                  <c:v>0.20800000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6868629150101524</c:v>
+                  <c:v>0.38139278553756395</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70762395692965985</c:v>
+                  <c:v>0.45820864063974154</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.72</c:v>
+                  <c:v>0.504</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.72844582472000674</c:v>
+                  <c:v>0.53524955146402498</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.73468027352578191</c:v>
+                  <c:v>0.55831701204539308</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73952568431852372</c:v>
+                  <c:v>0.57624503197853749</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.74343145750507622</c:v>
+                  <c:v>0.59069639276878205</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.7466666666666667</c:v>
+                  <c:v>0.60266666666666668</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.74940355743730602</c:v>
+                  <c:v>0.61279316251803195</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.75175818486755785</c:v>
+                  <c:v>0.62150528400996397</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.75381197846482995</c:v>
+                  <c:v>0.62910432031987074</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.75562398430198174</c:v>
+                  <c:v>0.63580874191733217</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.75723820129401209</c:v>
+                  <c:v>0.64178134478784477</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.75868817764045426</c:v>
+                  <c:v>0.64714625726968067</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.76</c:v>
+                  <c:v>0.65200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.76119429999418675</c:v>
+                  <c:v>0.65641890997849095</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.76228763833671753</c:v>
+                  <c:v>0.66046426184585461</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.76329348258071017</c:v>
+                  <c:v>0.66418588554862745</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.76422291236000339</c:v>
+                  <c:v>0.66762477573201251</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.76508513756224128</c:v>
+                  <c:v>0.67081500898029256</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.76588788538310237</c:v>
+                  <c:v>0.67378517591747866</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.7666376937508681</c:v>
+                  <c:v>0.67655946687821178</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.76734013676289103</c:v>
+                  <c:v>0.67915850602269656</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.76800000000000002</c:v>
+                  <c:v>0.68159999999999998</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.76862141837789055</c:v>
+                  <c:v>0.68389924799819513</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.76920798564322002</c:v>
+                  <c:v>0.68606954687991384</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.76976284215926183</c:v>
+                  <c:v>0.68812251598926877</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.77028874589167173</c:v>
+                  <c:v>0.69006835979918535</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.77078813026639115</c:v>
+                  <c:v>0.69191608198564725</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.77126315167571602</c:v>
+                  <c:v>0.69367366120014928</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.77171572875253813</c:v>
+                  <c:v>0.69534819638439105</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.77214757504708842</c:v>
+                  <c:v>0.69694602767422698</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.77256022637719868</c:v>
+                  <c:v>0.69847283759563483</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.77295506384868751</c:v>
+                  <c:v>0.69993373624014366</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.77333333333333343</c:v>
+                  <c:v>0.70133333333333336</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.77369616203114289</c:v>
+                  <c:v>0.70267579951522852</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.774044572619078</c:v>
+                  <c:v>0.70396491869058864</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.77437949539118611</c:v>
+                  <c:v>0.70520413294738848</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.77470177871865298</c:v>
+                  <c:v>0.70639658125901605</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -456,124 +456,124 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>0.84000000000000008</c:v>
+                  <c:v>0.94799999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82828427124746196</c:v>
+                  <c:v>0.90465180361560904</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82309401076758504</c:v>
+                  <c:v>0.8854478398400647</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.82000000000000006</c:v>
+                  <c:v>0.874</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81788854381999831</c:v>
+                  <c:v>0.86618761213399376</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.81632993161855461</c:v>
+                  <c:v>0.86042074698865179</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8151185789203691</c:v>
+                  <c:v>0.85593874200536568</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.81414213562373094</c:v>
+                  <c:v>0.85232590180780454</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.81333333333333335</c:v>
+                  <c:v>0.84933333333333338</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.81264911064067358</c:v>
+                  <c:v>0.84680170937049204</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.81206045378311054</c:v>
+                  <c:v>0.84462367899750901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.81154700538379254</c:v>
+                  <c:v>0.84272391992003237</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.81109400392450459</c:v>
+                  <c:v>0.84104781452066701</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.81069044967649706</c:v>
+                  <c:v>0.83955466380303889</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.81032795558988646</c:v>
+                  <c:v>0.83821343568257989</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.81</c:v>
+                  <c:v>0.83700000000000008</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.80970142500145337</c:v>
+                  <c:v>0.83589527250537732</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.80942809041582064</c:v>
+                  <c:v>0.83488393453853638</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.80917662935482249</c:v>
+                  <c:v>0.83395352861284322</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.80894427190999918</c:v>
+                  <c:v>0.8330938060669969</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.80872871560943971</c:v>
+                  <c:v>0.83229624775492694</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.80852802865422446</c:v>
+                  <c:v>0.83155370602063039</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.80834057656228309</c:v>
+                  <c:v>0.83086013328044706</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.80816496580927732</c:v>
+                  <c:v>0.83021037349432592</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.80800000000000005</c:v>
+                  <c:v>0.8296</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.80784464540552736</c:v>
+                  <c:v>0.82902518800045133</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.80769800358919508</c:v>
+                  <c:v>0.8284826132800216</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.80755928946018463</c:v>
+                  <c:v>0.82796937100268286</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.80742781352708215</c:v>
+                  <c:v>0.82748291005020369</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.80730296743340224</c:v>
+                  <c:v>0.82702097950358822</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.80718421208107105</c:v>
+                  <c:v>0.82658158469996268</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.80707106781186555</c:v>
+                  <c:v>0.82616295090390235</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.80696310623822798</c:v>
+                  <c:v>0.82576349308144337</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.80685994340570044</c:v>
+                  <c:v>0.8253817906010914</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.80676123403782818</c:v>
+                  <c:v>0.82501656593996409</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.80666666666666675</c:v>
+                  <c:v>0.82466666666666666</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.80657595949221439</c:v>
+                  <c:v>0.8243310501211929</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.80648885684523053</c:v>
+                  <c:v>0.82400877032735287</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.8064051261522035</c:v>
+                  <c:v>0.82369896676315291</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.80632455532033676</c:v>
+                  <c:v>0.82340085468524604</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1008,124 +1008,124 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>-0.16000000000000003</c:v>
+                  <c:v>-0.59199999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.11313708498984765</c:v>
+                  <c:v>-0.41860721446243609</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-9.2376043070340197E-2</c:v>
+                  <c:v>-0.34179135936025851</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.0000000000000071E-2</c:v>
+                  <c:v>-0.29600000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-7.1554175279993304E-2</c:v>
+                  <c:v>-0.26475044853597507</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-6.5319726474218132E-2</c:v>
+                  <c:v>-0.24168298795460696</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-6.0474315681476321E-2</c:v>
+                  <c:v>-0.22375496802146255</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.6568542494923824E-2</c:v>
+                  <c:v>-0.20930360723121799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5.3333333333333344E-2</c:v>
+                  <c:v>-0.19733333333333336</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-5.0596442562694022E-2</c:v>
+                  <c:v>-0.18720683748196809</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-4.824181513244219E-2</c:v>
+                  <c:v>-0.17849471599003608</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-4.6188021535170098E-2</c:v>
+                  <c:v>-0.17089567968012931</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-4.4376015698018301E-2</c:v>
+                  <c:v>-0.16419125808266788</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-4.2761798705987952E-2</c:v>
+                  <c:v>-0.15821865521215528</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-4.131182235954578E-2</c:v>
+                  <c:v>-0.15285374273031938</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-4.0000000000000036E-2</c:v>
+                  <c:v>-0.14800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-3.8805700005813293E-2</c:v>
+                  <c:v>-0.14358109002150909</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-3.7712361663282512E-2</c:v>
+                  <c:v>-0.13953573815414544</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-3.6706517419289875E-2</c:v>
+                  <c:v>-0.13581411445137259</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-3.5777087639996652E-2</c:v>
+                  <c:v>-0.13237522426798753</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-3.4914862437758765E-2</c:v>
+                  <c:v>-0.12918499101970748</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-3.4112114616897671E-2</c:v>
+                  <c:v>-0.12621482408252138</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-3.3362306249131946E-2</c:v>
+                  <c:v>-0.12344053312178827</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-3.265986323710901E-2</c:v>
+                  <c:v>-0.12084149397730348</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-3.2000000000000028E-2</c:v>
+                  <c:v>-0.11840000000000006</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-3.1378581622109492E-2</c:v>
+                  <c:v>-0.11610075200180492</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-3.0792014356780029E-2</c:v>
+                  <c:v>-0.11393045312008621</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-3.0237157840738216E-2</c:v>
+                  <c:v>-0.11187748401073128</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-2.9711254108328311E-2</c:v>
+                  <c:v>-0.1099316402008147</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-2.9211869733608897E-2</c:v>
+                  <c:v>-0.1080839180143528</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-2.8736848324284026E-2</c:v>
+                  <c:v>-0.10632633879985076</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-2.8284271247461912E-2</c:v>
+                  <c:v>-0.104651803615609</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-2.7852424952911625E-2</c:v>
+                  <c:v>-0.10305397232577307</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-2.7439773622801367E-2</c:v>
+                  <c:v>-0.10152716240436521</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-2.7044936151312537E-2</c:v>
+                  <c:v>-0.10006626375985639</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-2.6666666666666616E-2</c:v>
+                  <c:v>-9.866666666666668E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-2.6303837968857158E-2</c:v>
+                  <c:v>-9.7324200484771528E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-2.5955427380922047E-2</c:v>
+                  <c:v>-9.6035081309411408E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-2.5620504608813932E-2</c:v>
+                  <c:v>-9.479586705261156E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-2.5298221281347066E-2</c:v>
+                  <c:v>-9.360341874098399E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1170,124 +1170,124 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>4.0000000000000036E-2</c:v>
+                  <c:v>0.14799999999999991</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8284271247461912E-2</c:v>
+                  <c:v>0.104651803615609</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3094010767584994E-2</c:v>
+                  <c:v>8.5447839840064654E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0000000000000018E-2</c:v>
+                  <c:v>7.3999999999999955E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.788854381999827E-2</c:v>
+                  <c:v>6.6187612133993712E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6329931618554561E-2</c:v>
+                  <c:v>6.0420746988651741E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5118578920369052E-2</c:v>
+                  <c:v>5.5938742005365638E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.41421356237309E-2</c:v>
+                  <c:v>5.2325901807804498E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3333333333333308E-2</c:v>
+                  <c:v>4.933333333333334E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2649110640673533E-2</c:v>
+                  <c:v>4.6801709370491995E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.2060453783110492E-2</c:v>
+                  <c:v>4.4623678997508964E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.1547005383792497E-2</c:v>
+                  <c:v>4.2723919920032327E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1094003924504547E-2</c:v>
+                  <c:v>4.104781452066697E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0690449676497016E-2</c:v>
+                  <c:v>3.9554663803038848E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0327955589886417E-2</c:v>
+                  <c:v>3.8213435682579844E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0000000000000009E-2</c:v>
+                  <c:v>3.7000000000000033E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.7014250014533232E-3</c:v>
+                  <c:v>3.5895272505377274E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.4280904158206003E-3</c:v>
+                  <c:v>3.4883934538536332E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.1766293548224409E-3</c:v>
+                  <c:v>3.3953528612843176E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.9442719099991352E-3</c:v>
+                  <c:v>3.3093806066996856E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.7287156094396634E-3</c:v>
+                  <c:v>3.2296247754926899E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.5280286542244177E-3</c:v>
+                  <c:v>3.1553706020630345E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.3405765622830419E-3</c:v>
+                  <c:v>3.0860133280447011E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.1649658092772803E-3</c:v>
+                  <c:v>3.0210373494325871E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.0000000000000071E-3</c:v>
+                  <c:v>2.959999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.8446454055273174E-3</c:v>
+                  <c:v>2.9025188000451285E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.6980035891950349E-3</c:v>
+                  <c:v>2.8482613280021551E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.5592894601845817E-3</c:v>
+                  <c:v>2.7969371002682819E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.4278135270821055E-3</c:v>
+                  <c:v>2.7482910050203646E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.3029674334021966E-3</c:v>
+                  <c:v>2.7020979503588172E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.1842120810710064E-3</c:v>
+                  <c:v>2.6581584699962635E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.0710678118655057E-3</c:v>
+                  <c:v>2.6162950903902304E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.9631062382279341E-3</c:v>
+                  <c:v>2.5763493081443323E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.8599434057003972E-3</c:v>
+                  <c:v>2.5381790601091359E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.7612340378281344E-3</c:v>
+                  <c:v>2.5016565939964042E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.6666666666667096E-3</c:v>
+                  <c:v>2.4666666666666615E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.5759594922143449E-3</c:v>
+                  <c:v>2.4331050121192854E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.488856845230484E-3</c:v>
+                  <c:v>2.4008770327352824E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.4051261522034553E-3</c:v>
+                  <c:v>2.3698966763152862E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.3245553203367111E-3</c:v>
+                  <c:v>2.3400854685245998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2770,8 +2770,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -3785,7 +3785,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -4514,7 +4514,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4557,19 +4557,19 @@
       </c>
       <c r="B2" s="4">
         <f t="shared" ref="B2:B21" si="0">$G$3 - $G$3*($H$3 / SQRT(A2))</f>
-        <v>0.64</v>
+        <v>0.20800000000000007</v>
       </c>
       <c r="C2" s="4">
         <f t="shared" ref="C2:C21" si="1">$G$3 +(1- $G$3)*($H$3 / SQRT(A2))</f>
-        <v>0.84000000000000008</v>
+        <v>0.94799999999999995</v>
       </c>
       <c r="D2" s="4">
         <f>B2-$G$3</f>
-        <v>-0.16000000000000003</v>
+        <v>-0.59199999999999997</v>
       </c>
       <c r="E2" s="4">
         <f>C2-$G$3</f>
-        <v>4.0000000000000036E-2</v>
+        <v>0.14799999999999991</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>0</v>
@@ -4588,29 +4588,29 @@
       </c>
       <c r="B3" s="4">
         <f t="shared" si="0"/>
-        <v>0.6868629150101524</v>
+        <v>0.38139278553756395</v>
       </c>
       <c r="C3" s="4">
         <f t="shared" si="1"/>
-        <v>0.82828427124746196</v>
+        <v>0.90465180361560904</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3:D21" si="2">B3-$G$3</f>
-        <v>-0.11313708498984765</v>
+        <v>-0.41860721446243609</v>
       </c>
       <c r="E3" s="4">
         <f t="shared" ref="E3:E21" si="3">C3-$G$3</f>
-        <v>2.8284271247461912E-2</v>
+        <v>0.104651803615609</v>
       </c>
       <c r="G3">
         <v>0.8</v>
       </c>
       <c r="H3">
-        <v>0.2</v>
+        <v>0.74</v>
       </c>
       <c r="I3">
         <f xml:space="preserve"> -H3</f>
-        <v>-0.2</v>
+        <v>-0.74</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4620,19 +4620,19 @@
       </c>
       <c r="B4" s="4">
         <f t="shared" si="0"/>
-        <v>0.70762395692965985</v>
+        <v>0.45820864063974154</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" si="1"/>
-        <v>0.82309401076758504</v>
+        <v>0.8854478398400647</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="2"/>
-        <v>-9.2376043070340197E-2</v>
+        <v>-0.34179135936025851</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="3"/>
-        <v>2.3094010767584994E-2</v>
+        <v>8.5447839840064654E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -4642,19 +4642,19 @@
       </c>
       <c r="B5" s="4">
         <f t="shared" si="0"/>
-        <v>0.72</v>
+        <v>0.504</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="1"/>
-        <v>0.82000000000000006</v>
+        <v>0.874</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="2"/>
-        <v>-8.0000000000000071E-2</v>
+        <v>-0.29600000000000004</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="3"/>
-        <v>2.0000000000000018E-2</v>
+        <v>7.3999999999999955E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -4664,19 +4664,19 @@
       </c>
       <c r="B6" s="4">
         <f t="shared" si="0"/>
-        <v>0.72844582472000674</v>
+        <v>0.53524955146402498</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="1"/>
-        <v>0.81788854381999831</v>
+        <v>0.86618761213399376</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="2"/>
-        <v>-7.1554175279993304E-2</v>
+        <v>-0.26475044853597507</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="3"/>
-        <v>1.788854381999827E-2</v>
+        <v>6.6187612133993712E-2</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -4687,19 +4687,19 @@
       </c>
       <c r="B7" s="4">
         <f t="shared" si="0"/>
-        <v>0.73468027352578191</v>
+        <v>0.55831701204539308</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="1"/>
-        <v>0.81632993161855461</v>
+        <v>0.86042074698865179</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="2"/>
-        <v>-6.5319726474218132E-2</v>
+        <v>-0.24168298795460696</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="3"/>
-        <v>1.6329931618554561E-2</v>
+        <v>6.0420746988651741E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4709,19 +4709,19 @@
       </c>
       <c r="B8" s="4">
         <f t="shared" si="0"/>
-        <v>0.73952568431852372</v>
+        <v>0.57624503197853749</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="1"/>
-        <v>0.8151185789203691</v>
+        <v>0.85593874200536568</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="2"/>
-        <v>-6.0474315681476321E-2</v>
+        <v>-0.22375496802146255</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="3"/>
-        <v>1.5118578920369052E-2</v>
+        <v>5.5938742005365638E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -4731,19 +4731,19 @@
       </c>
       <c r="B9" s="4">
         <f t="shared" si="0"/>
-        <v>0.74343145750507622</v>
+        <v>0.59069639276878205</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="1"/>
-        <v>0.81414213562373094</v>
+        <v>0.85232590180780454</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="2"/>
-        <v>-5.6568542494923824E-2</v>
+        <v>-0.20930360723121799</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="3"/>
-        <v>1.41421356237309E-2</v>
+        <v>5.2325901807804498E-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -4753,19 +4753,19 @@
       </c>
       <c r="B10" s="4">
         <f t="shared" si="0"/>
-        <v>0.7466666666666667</v>
+        <v>0.60266666666666668</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="1"/>
-        <v>0.81333333333333335</v>
+        <v>0.84933333333333338</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="2"/>
-        <v>-5.3333333333333344E-2</v>
+        <v>-0.19733333333333336</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="3"/>
-        <v>1.3333333333333308E-2</v>
+        <v>4.933333333333334E-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -4775,19 +4775,19 @@
       </c>
       <c r="B11" s="4">
         <f t="shared" si="0"/>
-        <v>0.74940355743730602</v>
+        <v>0.61279316251803195</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="1"/>
-        <v>0.81264911064067358</v>
+        <v>0.84680170937049204</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="2"/>
-        <v>-5.0596442562694022E-2</v>
+        <v>-0.18720683748196809</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="3"/>
-        <v>1.2649110640673533E-2</v>
+        <v>4.6801709370491995E-2</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -4798,19 +4798,19 @@
       </c>
       <c r="B12" s="4">
         <f t="shared" si="0"/>
-        <v>0.75175818486755785</v>
+        <v>0.62150528400996397</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="1"/>
-        <v>0.81206045378311054</v>
+        <v>0.84462367899750901</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="2"/>
-        <v>-4.824181513244219E-2</v>
+        <v>-0.17849471599003608</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="3"/>
-        <v>1.2060453783110492E-2</v>
+        <v>4.4623678997508964E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4820,19 +4820,19 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" si="0"/>
-        <v>0.75381197846482995</v>
+        <v>0.62910432031987074</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="1"/>
-        <v>0.81154700538379254</v>
+        <v>0.84272391992003237</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="2"/>
-        <v>-4.6188021535170098E-2</v>
+        <v>-0.17089567968012931</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="3"/>
-        <v>1.1547005383792497E-2</v>
+        <v>4.2723919920032327E-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -4842,19 +4842,19 @@
       </c>
       <c r="B14" s="4">
         <f t="shared" si="0"/>
-        <v>0.75562398430198174</v>
+        <v>0.63580874191733217</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="1"/>
-        <v>0.81109400392450459</v>
+        <v>0.84104781452066701</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="2"/>
-        <v>-4.4376015698018301E-2</v>
+        <v>-0.16419125808266788</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="3"/>
-        <v>1.1094003924504547E-2</v>
+        <v>4.104781452066697E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -4864,19 +4864,19 @@
       </c>
       <c r="B15" s="4">
         <f t="shared" si="0"/>
-        <v>0.75723820129401209</v>
+        <v>0.64178134478784477</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="1"/>
-        <v>0.81069044967649706</v>
+        <v>0.83955466380303889</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="2"/>
-        <v>-4.2761798705987952E-2</v>
+        <v>-0.15821865521215528</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="3"/>
-        <v>1.0690449676497016E-2</v>
+        <v>3.9554663803038848E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4886,19 +4886,19 @@
       </c>
       <c r="B16" s="4">
         <f t="shared" si="0"/>
-        <v>0.75868817764045426</v>
+        <v>0.64714625726968067</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="1"/>
-        <v>0.81032795558988646</v>
+        <v>0.83821343568257989</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="2"/>
-        <v>-4.131182235954578E-2</v>
+        <v>-0.15285374273031938</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="3"/>
-        <v>1.0327955589886417E-2</v>
+        <v>3.8213435682579844E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -4908,19 +4908,19 @@
       </c>
       <c r="B17" s="4">
         <f t="shared" si="0"/>
-        <v>0.76</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="1"/>
-        <v>0.81</v>
+        <v>0.83700000000000008</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="2"/>
-        <v>-4.0000000000000036E-2</v>
+        <v>-0.14800000000000002</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="3"/>
-        <v>1.0000000000000009E-2</v>
+        <v>3.7000000000000033E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -4930,19 +4930,19 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" si="0"/>
-        <v>0.76119429999418675</v>
+        <v>0.65641890997849095</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="1"/>
-        <v>0.80970142500145337</v>
+        <v>0.83589527250537732</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="2"/>
-        <v>-3.8805700005813293E-2</v>
+        <v>-0.14358109002150909</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="3"/>
-        <v>9.7014250014533232E-3</v>
+        <v>3.5895272505377274E-2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -4952,19 +4952,19 @@
       </c>
       <c r="B19" s="4">
         <f t="shared" si="0"/>
-        <v>0.76228763833671753</v>
+        <v>0.66046426184585461</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="1"/>
-        <v>0.80942809041582064</v>
+        <v>0.83488393453853638</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="2"/>
-        <v>-3.7712361663282512E-2</v>
+        <v>-0.13953573815414544</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="3"/>
-        <v>9.4280904158206003E-3</v>
+        <v>3.4883934538536332E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -4974,19 +4974,19 @@
       </c>
       <c r="B20" s="4">
         <f t="shared" si="0"/>
-        <v>0.76329348258071017</v>
+        <v>0.66418588554862745</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>0.80917662935482249</v>
+        <v>0.83395352861284322</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="2"/>
-        <v>-3.6706517419289875E-2</v>
+        <v>-0.13581411445137259</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="3"/>
-        <v>9.1766293548224409E-3</v>
+        <v>3.3953528612843176E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -4996,19 +4996,19 @@
       </c>
       <c r="B21" s="4">
         <f t="shared" si="0"/>
-        <v>0.76422291236000339</v>
+        <v>0.66762477573201251</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>0.80894427190999918</v>
+        <v>0.8330938060669969</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="2"/>
-        <v>-3.5777087639996652E-2</v>
+        <v>-0.13237522426798753</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="3"/>
-        <v>8.9442719099991352E-3</v>
+        <v>3.3093806066996856E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -5018,19 +5018,19 @@
       </c>
       <c r="B22" s="4">
         <f t="shared" ref="B22:B41" si="5">$G$3 - $G$3*($H$3 / SQRT(A22))</f>
-        <v>0.76508513756224128</v>
+        <v>0.67081500898029256</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" ref="C22:C41" si="6">$G$3 +(1- $G$3)*($H$3 / SQRT(A22))</f>
-        <v>0.80872871560943971</v>
+        <v>0.83229624775492694</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" ref="D22:D41" si="7">B22-$G$3</f>
-        <v>-3.4914862437758765E-2</v>
+        <v>-0.12918499101970748</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" ref="E22:E41" si="8">C22-$G$3</f>
-        <v>8.7287156094396634E-3</v>
+        <v>3.2296247754926899E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -5040,19 +5040,19 @@
       </c>
       <c r="B23" s="4">
         <f t="shared" si="5"/>
-        <v>0.76588788538310237</v>
+        <v>0.67378517591747866</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="6"/>
-        <v>0.80852802865422446</v>
+        <v>0.83155370602063039</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="7"/>
-        <v>-3.4112114616897671E-2</v>
+        <v>-0.12621482408252138</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="8"/>
-        <v>8.5280286542244177E-3</v>
+        <v>3.1553706020630345E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -5062,19 +5062,19 @@
       </c>
       <c r="B24" s="4">
         <f t="shared" si="5"/>
-        <v>0.7666376937508681</v>
+        <v>0.67655946687821178</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="6"/>
-        <v>0.80834057656228309</v>
+        <v>0.83086013328044706</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="7"/>
-        <v>-3.3362306249131946E-2</v>
+        <v>-0.12344053312178827</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="8"/>
-        <v>8.3405765622830419E-3</v>
+        <v>3.0860133280447011E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -5084,19 +5084,19 @@
       </c>
       <c r="B25" s="4">
         <f t="shared" si="5"/>
-        <v>0.76734013676289103</v>
+        <v>0.67915850602269656</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="6"/>
-        <v>0.80816496580927732</v>
+        <v>0.83021037349432592</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="7"/>
-        <v>-3.265986323710901E-2</v>
+        <v>-0.12084149397730348</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="8"/>
-        <v>8.1649658092772803E-3</v>
+        <v>3.0210373494325871E-2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -5106,19 +5106,19 @@
       </c>
       <c r="B26" s="4">
         <f t="shared" si="5"/>
-        <v>0.76800000000000002</v>
+        <v>0.68159999999999998</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="6"/>
-        <v>0.80800000000000005</v>
+        <v>0.8296</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="7"/>
-        <v>-3.2000000000000028E-2</v>
+        <v>-0.11840000000000006</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="8"/>
-        <v>8.0000000000000071E-3</v>
+        <v>2.959999999999996E-2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -5128,19 +5128,19 @@
       </c>
       <c r="B27" s="4">
         <f t="shared" si="5"/>
-        <v>0.76862141837789055</v>
+        <v>0.68389924799819513</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="6"/>
-        <v>0.80784464540552736</v>
+        <v>0.82902518800045133</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="7"/>
-        <v>-3.1378581622109492E-2</v>
+        <v>-0.11610075200180492</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="8"/>
-        <v>7.8446454055273174E-3</v>
+        <v>2.9025188000451285E-2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -5150,19 +5150,19 @@
       </c>
       <c r="B28" s="4">
         <f t="shared" si="5"/>
-        <v>0.76920798564322002</v>
+        <v>0.68606954687991384</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="6"/>
-        <v>0.80769800358919508</v>
+        <v>0.8284826132800216</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="7"/>
-        <v>-3.0792014356780029E-2</v>
+        <v>-0.11393045312008621</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" si="8"/>
-        <v>7.6980035891950349E-3</v>
+        <v>2.8482613280021551E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -5172,19 +5172,19 @@
       </c>
       <c r="B29" s="4">
         <f t="shared" si="5"/>
-        <v>0.76976284215926183</v>
+        <v>0.68812251598926877</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="6"/>
-        <v>0.80755928946018463</v>
+        <v>0.82796937100268286</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="7"/>
-        <v>-3.0237157840738216E-2</v>
+        <v>-0.11187748401073128</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="8"/>
-        <v>7.5592894601845817E-3</v>
+        <v>2.7969371002682819E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -5194,19 +5194,19 @@
       </c>
       <c r="B30" s="4">
         <f t="shared" si="5"/>
-        <v>0.77028874589167173</v>
+        <v>0.69006835979918535</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="6"/>
-        <v>0.80742781352708215</v>
+        <v>0.82748291005020369</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="7"/>
-        <v>-2.9711254108328311E-2</v>
+        <v>-0.1099316402008147</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="8"/>
-        <v>7.4278135270821055E-3</v>
+        <v>2.7482910050203646E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -5216,19 +5216,19 @@
       </c>
       <c r="B31" s="4">
         <f t="shared" si="5"/>
-        <v>0.77078813026639115</v>
+        <v>0.69191608198564725</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="6"/>
-        <v>0.80730296743340224</v>
+        <v>0.82702097950358822</v>
       </c>
       <c r="D31" s="4">
         <f t="shared" si="7"/>
-        <v>-2.9211869733608897E-2</v>
+        <v>-0.1080839180143528</v>
       </c>
       <c r="E31" s="4">
         <f t="shared" si="8"/>
-        <v>7.3029674334021966E-3</v>
+        <v>2.7020979503588172E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -5238,19 +5238,19 @@
       </c>
       <c r="B32" s="4">
         <f t="shared" si="5"/>
-        <v>0.77126315167571602</v>
+        <v>0.69367366120014928</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="6"/>
-        <v>0.80718421208107105</v>
+        <v>0.82658158469996268</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="7"/>
-        <v>-2.8736848324284026E-2</v>
+        <v>-0.10632633879985076</v>
       </c>
       <c r="E32" s="4">
         <f t="shared" si="8"/>
-        <v>7.1842120810710064E-3</v>
+        <v>2.6581584699962635E-2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -5260,19 +5260,19 @@
       </c>
       <c r="B33" s="4">
         <f t="shared" si="5"/>
-        <v>0.77171572875253813</v>
+        <v>0.69534819638439105</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="6"/>
-        <v>0.80707106781186555</v>
+        <v>0.82616295090390235</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="7"/>
-        <v>-2.8284271247461912E-2</v>
+        <v>-0.104651803615609</v>
       </c>
       <c r="E33" s="4">
         <f t="shared" si="8"/>
-        <v>7.0710678118655057E-3</v>
+        <v>2.6162950903902304E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -5282,19 +5282,19 @@
       </c>
       <c r="B34" s="4">
         <f t="shared" si="5"/>
-        <v>0.77214757504708842</v>
+        <v>0.69694602767422698</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="6"/>
-        <v>0.80696310623822798</v>
+        <v>0.82576349308144337</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="7"/>
-        <v>-2.7852424952911625E-2</v>
+        <v>-0.10305397232577307</v>
       </c>
       <c r="E34" s="4">
         <f t="shared" si="8"/>
-        <v>6.9631062382279341E-3</v>
+        <v>2.5763493081443323E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -5304,19 +5304,19 @@
       </c>
       <c r="B35" s="4">
         <f t="shared" si="5"/>
-        <v>0.77256022637719868</v>
+        <v>0.69847283759563483</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="6"/>
-        <v>0.80685994340570044</v>
+        <v>0.8253817906010914</v>
       </c>
       <c r="D35" s="4">
         <f t="shared" si="7"/>
-        <v>-2.7439773622801367E-2</v>
+        <v>-0.10152716240436521</v>
       </c>
       <c r="E35" s="4">
         <f t="shared" si="8"/>
-        <v>6.8599434057003972E-3</v>
+        <v>2.5381790601091359E-2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -5326,19 +5326,19 @@
       </c>
       <c r="B36" s="4">
         <f t="shared" si="5"/>
-        <v>0.77295506384868751</v>
+        <v>0.69993373624014366</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="6"/>
-        <v>0.80676123403782818</v>
+        <v>0.82501656593996409</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="7"/>
-        <v>-2.7044936151312537E-2</v>
+        <v>-0.10006626375985639</v>
       </c>
       <c r="E36" s="4">
         <f t="shared" si="8"/>
-        <v>6.7612340378281344E-3</v>
+        <v>2.5016565939964042E-2</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -5348,19 +5348,19 @@
       </c>
       <c r="B37" s="4">
         <f t="shared" si="5"/>
-        <v>0.77333333333333343</v>
+        <v>0.70133333333333336</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="6"/>
-        <v>0.80666666666666675</v>
+        <v>0.82466666666666666</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" si="7"/>
-        <v>-2.6666666666666616E-2</v>
+        <v>-9.866666666666668E-2</v>
       </c>
       <c r="E37" s="4">
         <f t="shared" si="8"/>
-        <v>6.6666666666667096E-3</v>
+        <v>2.4666666666666615E-2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -5370,19 +5370,19 @@
       </c>
       <c r="B38" s="4">
         <f t="shared" si="5"/>
-        <v>0.77369616203114289</v>
+        <v>0.70267579951522852</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="6"/>
-        <v>0.80657595949221439</v>
+        <v>0.8243310501211929</v>
       </c>
       <c r="D38" s="4">
         <f t="shared" si="7"/>
-        <v>-2.6303837968857158E-2</v>
+        <v>-9.7324200484771528E-2</v>
       </c>
       <c r="E38" s="4">
         <f t="shared" si="8"/>
-        <v>6.5759594922143449E-3</v>
+        <v>2.4331050121192854E-2</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -5392,19 +5392,19 @@
       </c>
       <c r="B39" s="4">
         <f t="shared" si="5"/>
-        <v>0.774044572619078</v>
+        <v>0.70396491869058864</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="6"/>
-        <v>0.80648885684523053</v>
+        <v>0.82400877032735287</v>
       </c>
       <c r="D39" s="4">
         <f t="shared" si="7"/>
-        <v>-2.5955427380922047E-2</v>
+        <v>-9.6035081309411408E-2</v>
       </c>
       <c r="E39" s="4">
         <f t="shared" si="8"/>
-        <v>6.488856845230484E-3</v>
+        <v>2.4008770327352824E-2</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -5414,19 +5414,19 @@
       </c>
       <c r="B40" s="4">
         <f t="shared" si="5"/>
-        <v>0.77437949539118611</v>
+        <v>0.70520413294738848</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="6"/>
-        <v>0.8064051261522035</v>
+        <v>0.82369896676315291</v>
       </c>
       <c r="D40" s="4">
         <f t="shared" si="7"/>
-        <v>-2.5620504608813932E-2</v>
+        <v>-9.479586705261156E-2</v>
       </c>
       <c r="E40" s="4">
         <f t="shared" si="8"/>
-        <v>6.4051261522034553E-3</v>
+        <v>2.3698966763152862E-2</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -5436,19 +5436,19 @@
       </c>
       <c r="B41" s="4">
         <f t="shared" si="5"/>
-        <v>0.77470177871865298</v>
+        <v>0.70639658125901605</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="6"/>
-        <v>0.80632455532033676</v>
+        <v>0.82340085468524604</v>
       </c>
       <c r="D41" s="4">
         <f t="shared" si="7"/>
-        <v>-2.5298221281347066E-2</v>
+        <v>-9.360341874098399E-2</v>
       </c>
       <c r="E41" s="4">
         <f t="shared" si="8"/>
-        <v>6.3245553203367111E-3</v>
+        <v>2.3400854685245998E-2</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>